<commit_message>
[WIP] Fix Hawaii dynamic case, but failed
</commit_message>
<xml_diff>
--- a/demo/hawaii/Hawaii40.xlsx
+++ b/demo/hawaii/Hawaii40.xlsx
@@ -9112,10 +9112,10 @@
         <v>0.7</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>1.98019801980198</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>-1.98019801980198</v>
       </c>
       <c r="V2">
         <v>0.8</v>
@@ -9186,10 +9186,10 @@
         <v>0.7</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>6.17283950617284</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>-6.17283950617284</v>
       </c>
       <c r="V3">
         <v>0.8</v>
@@ -9260,10 +9260,10 @@
         <v>0.7</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>4.545454545454546</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>-4.545454545454546</v>
       </c>
       <c r="V4">
         <v>0.8</v>
@@ -9334,10 +9334,10 @@
         <v>0.7</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>8.928571428571429</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>-8.928571428571429</v>
       </c>
       <c r="V5">
         <v>0.8</v>
@@ -9408,10 +9408,10 @@
         <v>0.7</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>3.03030303030303</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>-3.03030303030303</v>
       </c>
       <c r="V6">
         <v>0.8</v>
@@ -9482,10 +9482,10 @@
         <v>0.7</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>3.289473684210527</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>-3.289473684210527</v>
       </c>
       <c r="V7">
         <v>0.8</v>
@@ -9556,10 +9556,10 @@
         <v>0.7</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>1.855287569573284</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>-1.855287569573284</v>
       </c>
       <c r="V8">
         <v>0.8</v>
@@ -9630,10 +9630,10 @@
         <v>0.7</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>1.317523056653491</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>-1.317523056653491</v>
       </c>
       <c r="V9">
         <v>0.8</v>
@@ -9704,10 +9704,10 @@
         <v>0.7</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>3.289473684210527</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>-3.289473684210527</v>
       </c>
       <c r="V10">
         <v>0.8</v>
@@ -9958,10 +9958,10 @@
         <v>5</v>
       </c>
       <c r="R2">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="S2">
-        <v>-1.1</v>
+        <v>-999</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -9979,16 +9979,16 @@
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>0.436</v>
+        <v>999</v>
       </c>
       <c r="Z2">
-        <v>-0.436</v>
+        <v>-999</v>
       </c>
       <c r="AA2">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="AB2">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -10003,7 +10003,7 @@
         <v>5</v>
       </c>
       <c r="AG2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH2">
         <v>0.02</v>
@@ -10015,13 +10015,13 @@
         <v>-99</v>
       </c>
       <c r="AK2">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="AL2">
         <v>0</v>
       </c>
       <c r="AM2">
-        <v>1.3</v>
+        <v>1978.217821782178</v>
       </c>
       <c r="AN2">
         <v>0.026</v>
@@ -10128,10 +10128,10 @@
         <v>5</v>
       </c>
       <c r="R3">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="S3">
-        <v>-1.1</v>
+        <v>-999</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -10149,16 +10149,16 @@
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>0.436</v>
+        <v>999</v>
       </c>
       <c r="Z3">
-        <v>-0.436</v>
+        <v>-999</v>
       </c>
       <c r="AA3">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="AB3">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="AC3">
         <v>0</v>
@@ -10173,7 +10173,7 @@
         <v>5</v>
       </c>
       <c r="AG3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH3">
         <v>0.02</v>
@@ -10185,13 +10185,13 @@
         <v>-99</v>
       </c>
       <c r="AK3">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="AL3">
         <v>0</v>
       </c>
       <c r="AM3">
-        <v>1.3</v>
+        <v>1978.217821782178</v>
       </c>
       <c r="AN3">
         <v>0.039</v>
@@ -10298,10 +10298,10 @@
         <v>5</v>
       </c>
       <c r="R4">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="S4">
-        <v>-1.1</v>
+        <v>-999</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -10319,16 +10319,16 @@
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>0.436</v>
+        <v>999</v>
       </c>
       <c r="Z4">
-        <v>-0.436</v>
+        <v>-999</v>
       </c>
       <c r="AA4">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="AB4">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -10343,7 +10343,7 @@
         <v>5</v>
       </c>
       <c r="AG4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH4">
         <v>0.02</v>
@@ -10355,13 +10355,13 @@
         <v>-99</v>
       </c>
       <c r="AK4">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="AL4">
         <v>0</v>
       </c>
       <c r="AM4">
-        <v>1.3</v>
+        <v>4540.909090909092</v>
       </c>
       <c r="AN4">
         <v>0.029</v>
@@ -10468,10 +10468,10 @@
         <v>5</v>
       </c>
       <c r="R5">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="S5">
-        <v>-1.1</v>
+        <v>-999</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -10489,16 +10489,16 @@
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>0.436</v>
+        <v>999</v>
       </c>
       <c r="Z5">
-        <v>-0.436</v>
+        <v>-999</v>
       </c>
       <c r="AA5">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="AB5">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -10513,7 +10513,7 @@
         <v>5</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH5">
         <v>0.02</v>
@@ -10525,13 +10525,13 @@
         <v>-99</v>
       </c>
       <c r="AK5">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="AL5">
         <v>0</v>
       </c>
       <c r="AM5">
-        <v>1.3</v>
+        <v>4540.909090909092</v>
       </c>
       <c r="AN5">
         <v>0.03</v>
@@ -10638,10 +10638,10 @@
         <v>5</v>
       </c>
       <c r="R6">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="S6">
-        <v>-1.1</v>
+        <v>-999</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -10659,16 +10659,16 @@
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>0.436</v>
+        <v>999</v>
       </c>
       <c r="Z6">
-        <v>-0.436</v>
+        <v>-999</v>
       </c>
       <c r="AA6">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="AB6">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -10683,7 +10683,7 @@
         <v>5</v>
       </c>
       <c r="AG6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6">
         <v>0.02</v>
@@ -10695,13 +10695,13 @@
         <v>-99</v>
       </c>
       <c r="AK6">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="AL6">
         <v>0</v>
       </c>
       <c r="AM6">
-        <v>1.3</v>
+        <v>3027.272727272727</v>
       </c>
       <c r="AN6">
         <v>0.025</v>
@@ -10808,10 +10808,10 @@
         <v>5</v>
       </c>
       <c r="R7">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="S7">
-        <v>-1.1</v>
+        <v>-999</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -10829,16 +10829,16 @@
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>0.436</v>
+        <v>999</v>
       </c>
       <c r="Z7">
-        <v>-0.436</v>
+        <v>-999</v>
       </c>
       <c r="AA7">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="AB7">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -10853,7 +10853,7 @@
         <v>5</v>
       </c>
       <c r="AG7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH7">
         <v>0.02</v>
@@ -10865,13 +10865,13 @@
         <v>-99</v>
       </c>
       <c r="AK7">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="AL7">
         <v>0</v>
       </c>
       <c r="AM7">
-        <v>1.3</v>
+        <v>3027.272727272727</v>
       </c>
       <c r="AN7">
         <v>0.026</v>
@@ -10978,10 +10978,10 @@
         <v>5</v>
       </c>
       <c r="R8">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="S8">
-        <v>-1.1</v>
+        <v>-999</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -10999,16 +10999,16 @@
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>0.436</v>
+        <v>999</v>
       </c>
       <c r="Z8">
-        <v>-0.436</v>
+        <v>-999</v>
       </c>
       <c r="AA8">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="AB8">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -11023,7 +11023,7 @@
         <v>5</v>
       </c>
       <c r="AG8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH8">
         <v>0.02</v>
@@ -11035,13 +11035,13 @@
         <v>-99</v>
       </c>
       <c r="AK8">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="AL8">
         <v>0</v>
       </c>
       <c r="AM8">
-        <v>1.3</v>
+        <v>1853.43228200371</v>
       </c>
       <c r="AN8">
         <v>0.026</v>
@@ -11148,10 +11148,10 @@
         <v>5</v>
       </c>
       <c r="R9">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="S9">
-        <v>-1.1</v>
+        <v>-999</v>
       </c>
       <c r="T9">
         <v>0</v>
@@ -11169,16 +11169,16 @@
         <v>0</v>
       </c>
       <c r="Y9">
-        <v>0.436</v>
+        <v>999</v>
       </c>
       <c r="Z9">
-        <v>-0.436</v>
+        <v>-999</v>
       </c>
       <c r="AA9">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="AB9">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -11193,7 +11193,7 @@
         <v>5</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9">
         <v>0.02</v>
@@ -11205,13 +11205,13 @@
         <v>-99</v>
       </c>
       <c r="AK9">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="AL9">
         <v>0</v>
       </c>
       <c r="AM9">
-        <v>1.3</v>
+        <v>1853.43228200371</v>
       </c>
       <c r="AN9">
         <v>0.029</v>
@@ -11318,10 +11318,10 @@
         <v>5</v>
       </c>
       <c r="R10">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="S10">
-        <v>-1.1</v>
+        <v>-999</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -11339,16 +11339,16 @@
         <v>0</v>
       </c>
       <c r="Y10">
-        <v>0.436</v>
+        <v>999</v>
       </c>
       <c r="Z10">
-        <v>-0.436</v>
+        <v>-999</v>
       </c>
       <c r="AA10">
-        <v>1.1</v>
+        <v>999</v>
       </c>
       <c r="AB10">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -11363,7 +11363,7 @@
         <v>5</v>
       </c>
       <c r="AG10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
         <v>0.02</v>
@@ -11375,13 +11375,13 @@
         <v>-99</v>
       </c>
       <c r="AK10">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="AL10">
         <v>0</v>
       </c>
       <c r="AM10">
-        <v>1.3</v>
+        <v>3286.184210526316</v>
       </c>
       <c r="AN10">
         <v>0.025</v>

</xml_diff>